<commit_message>
Automatic start-date matching for (sub)tasks
</commit_message>
<xml_diff>
--- a/gantt.xlsx
+++ b/gantt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aniba\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0132A143-1E23-41F6-A0BD-231B4B75A2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86540085-AC41-417C-8286-DD4959AC1C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{DA0CE161-BB7D-4A4B-BBD7-0003F46AF39A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{DA0CE161-BB7D-4A4B-BBD7-0003F46AF39A}"/>
   </bookViews>
   <sheets>
     <sheet name="user guide" sheetId="8" r:id="rId1"/>
@@ -970,10 +970,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -982,6 +988,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" textRotation="90"/>
     </xf>
@@ -989,15 +998,6 @@
       <alignment vertical="top" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2261,7 +2261,7 @@
   </sheetPr>
   <dimension ref="A2:BP40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="CI14" sqref="CI14"/>
     </sheetView>
   </sheetViews>
@@ -2284,11 +2284,11 @@
       <c r="C2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="48">
+      <c r="D2" s="41">
         <v>45689</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
       <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:68" x14ac:dyDescent="0.35">
@@ -2296,11 +2296,11 @@
       <c r="C3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="49">
+      <c r="D3" s="42">
         <v>45961</v>
       </c>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:68" ht="5.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K4" s="33" cm="1">
@@ -2442,102 +2442,102 @@
       <c r="BP4" s="33"/>
     </row>
     <row r="5" spans="1:68" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="43" t="s">
+      <c r="C5" s="44"/>
+      <c r="D5" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43" t="s">
+      <c r="E5" s="45"/>
+      <c r="F5" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43" t="s">
+      <c r="G5" s="45"/>
+      <c r="H5" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="43" t="s">
+      <c r="J5" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="41" t="s">
+      <c r="K5" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="41"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="41"/>
-      <c r="U5" s="41"/>
-      <c r="V5" s="41"/>
-      <c r="W5" s="41"/>
-      <c r="X5" s="41"/>
-      <c r="Y5" s="41"/>
-      <c r="Z5" s="41"/>
-      <c r="AA5" s="41"/>
-      <c r="AB5" s="41"/>
-      <c r="AC5" s="41"/>
-      <c r="AD5" s="41"/>
-      <c r="AE5" s="41"/>
-      <c r="AF5" s="41"/>
-      <c r="AG5" s="41"/>
-      <c r="AH5" s="41"/>
-      <c r="AI5" s="41"/>
-      <c r="AJ5" s="41"/>
-      <c r="AK5" s="41"/>
-      <c r="AL5" s="41"/>
-      <c r="AM5" s="41"/>
-      <c r="AN5" s="41"/>
-      <c r="AO5" s="41"/>
-      <c r="AP5" s="41"/>
-      <c r="AQ5" s="41"/>
-      <c r="AR5" s="41"/>
-      <c r="AS5" s="41"/>
-      <c r="AT5" s="41"/>
-      <c r="AU5" s="41"/>
-      <c r="AV5" s="41"/>
-      <c r="AW5" s="41"/>
-      <c r="AX5" s="41"/>
-      <c r="AY5" s="41"/>
-      <c r="AZ5" s="41"/>
-      <c r="BA5" s="41"/>
-      <c r="BB5" s="41"/>
-      <c r="BC5" s="41"/>
-      <c r="BD5" s="41"/>
-      <c r="BE5" s="41"/>
-      <c r="BF5" s="41"/>
-      <c r="BG5" s="41"/>
-      <c r="BH5" s="41"/>
-      <c r="BI5" s="41"/>
-      <c r="BJ5" s="41"/>
-      <c r="BK5" s="41"/>
-      <c r="BL5" s="41"/>
-      <c r="BM5" s="41"/>
-      <c r="BN5" s="41"/>
-      <c r="BO5" s="41"/>
-      <c r="BP5" s="41"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="44"/>
+      <c r="S5" s="44"/>
+      <c r="T5" s="44"/>
+      <c r="U5" s="44"/>
+      <c r="V5" s="44"/>
+      <c r="W5" s="44"/>
+      <c r="X5" s="44"/>
+      <c r="Y5" s="44"/>
+      <c r="Z5" s="44"/>
+      <c r="AA5" s="44"/>
+      <c r="AB5" s="44"/>
+      <c r="AC5" s="44"/>
+      <c r="AD5" s="44"/>
+      <c r="AE5" s="44"/>
+      <c r="AF5" s="44"/>
+      <c r="AG5" s="44"/>
+      <c r="AH5" s="44"/>
+      <c r="AI5" s="44"/>
+      <c r="AJ5" s="44"/>
+      <c r="AK5" s="44"/>
+      <c r="AL5" s="44"/>
+      <c r="AM5" s="44"/>
+      <c r="AN5" s="44"/>
+      <c r="AO5" s="44"/>
+      <c r="AP5" s="44"/>
+      <c r="AQ5" s="44"/>
+      <c r="AR5" s="44"/>
+      <c r="AS5" s="44"/>
+      <c r="AT5" s="44"/>
+      <c r="AU5" s="44"/>
+      <c r="AV5" s="44"/>
+      <c r="AW5" s="44"/>
+      <c r="AX5" s="44"/>
+      <c r="AY5" s="44"/>
+      <c r="AZ5" s="44"/>
+      <c r="BA5" s="44"/>
+      <c r="BB5" s="44"/>
+      <c r="BC5" s="44"/>
+      <c r="BD5" s="44"/>
+      <c r="BE5" s="44"/>
+      <c r="BF5" s="44"/>
+      <c r="BG5" s="44"/>
+      <c r="BH5" s="44"/>
+      <c r="BI5" s="44"/>
+      <c r="BJ5" s="44"/>
+      <c r="BK5" s="44"/>
+      <c r="BL5" s="44"/>
+      <c r="BM5" s="44"/>
+      <c r="BN5" s="44"/>
+      <c r="BO5" s="44"/>
+      <c r="BP5" s="44"/>
     </row>
     <row r="6" spans="1:68" s="34" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="45"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
+      <c r="A6" s="48"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
       <c r="K6" s="1" t="str">
         <f>UPPER(IF(ISBLANK(K4), "", _xlfn.LET(
     _xlpm.date_of_previous_week, DATE(YEAR(D2),1,1) - WEEKDAY(DATE(YEAR(D2),1,1)) + 7*J4,
@@ -2780,7 +2780,7 @@
       </c>
     </row>
     <row r="7" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A7" s="46"/>
+      <c r="A7" s="49"/>
       <c r="B7" s="25"/>
       <c r="C7" s="26" t="s">
         <v>55</v>
@@ -3051,7 +3051,7 @@
       </c>
     </row>
     <row r="8" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A8" s="46"/>
+      <c r="A8" s="49"/>
       <c r="B8" s="25">
         <v>1</v>
       </c>
@@ -3322,7 +3322,7 @@
       </c>
     </row>
     <row r="9" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A9" s="46"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="25" t="s">
         <v>21</v>
       </c>
@@ -3582,7 +3582,7 @@
       </c>
     </row>
     <row r="10" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A10" s="46"/>
+      <c r="A10" s="49"/>
       <c r="B10" s="25" t="s">
         <v>22</v>
       </c>
@@ -3842,7 +3842,7 @@
       </c>
     </row>
     <row r="11" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A11" s="46"/>
+      <c r="A11" s="49"/>
       <c r="B11" s="25">
         <v>2</v>
       </c>
@@ -4122,7 +4122,7 @@
       </c>
     </row>
     <row r="12" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A12" s="46"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="25" t="s">
         <v>23</v>
       </c>
@@ -4391,7 +4391,7 @@
       </c>
     </row>
     <row r="13" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A13" s="46"/>
+      <c r="A13" s="49"/>
       <c r="B13" s="25" t="s">
         <v>24</v>
       </c>
@@ -4653,7 +4653,7 @@
       </c>
     </row>
     <row r="14" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A14" s="46"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="25" t="s">
         <v>25</v>
       </c>
@@ -4913,7 +4913,7 @@
       </c>
     </row>
     <row r="15" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A15" s="46"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="25" t="s">
         <v>26</v>
       </c>
@@ -5174,7 +5174,7 @@
       </c>
     </row>
     <row r="16" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A16" s="46"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="25" t="s">
         <v>27</v>
       </c>
@@ -5435,7 +5435,7 @@
       </c>
     </row>
     <row r="17" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A17" s="46"/>
+      <c r="A17" s="49"/>
       <c r="B17" s="25" t="s">
         <v>28</v>
       </c>
@@ -5696,7 +5696,7 @@
       </c>
     </row>
     <row r="18" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A18" s="46"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="25" t="s">
         <v>29</v>
       </c>
@@ -5957,7 +5957,7 @@
       </c>
     </row>
     <row r="19" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A19" s="46"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="25" t="s">
         <v>30</v>
       </c>
@@ -6218,7 +6218,7 @@
       </c>
     </row>
     <row r="20" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A20" s="46"/>
+      <c r="A20" s="49"/>
       <c r="B20" s="25" t="s">
         <v>31</v>
       </c>
@@ -6479,7 +6479,7 @@
       </c>
     </row>
     <row r="21" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A21" s="46"/>
+      <c r="A21" s="49"/>
       <c r="B21" s="25" t="s">
         <v>32</v>
       </c>
@@ -6740,7 +6740,7 @@
       </c>
     </row>
     <row r="22" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A22" s="46"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="25">
         <v>3</v>
       </c>
@@ -7001,7 +7001,7 @@
       </c>
     </row>
     <row r="23" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A23" s="46"/>
+      <c r="A23" s="49"/>
       <c r="B23" s="25" t="s">
         <v>34</v>
       </c>
@@ -7261,7 +7261,7 @@
       </c>
     </row>
     <row r="24" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A24" s="46"/>
+      <c r="A24" s="49"/>
       <c r="B24" s="25" t="s">
         <v>35</v>
       </c>
@@ -7521,7 +7521,7 @@
       </c>
     </row>
     <row r="25" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A25" s="46"/>
+      <c r="A25" s="49"/>
       <c r="B25" s="25" t="s">
         <v>36</v>
       </c>
@@ -7781,7 +7781,7 @@
       </c>
     </row>
     <row r="26" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A26" s="46"/>
+      <c r="A26" s="49"/>
       <c r="B26" s="25">
         <v>4</v>
       </c>
@@ -8042,7 +8042,7 @@
       </c>
     </row>
     <row r="27" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A27" s="46"/>
+      <c r="A27" s="49"/>
       <c r="B27" s="25" t="s">
         <v>37</v>
       </c>
@@ -8311,7 +8311,7 @@
       </c>
     </row>
     <row r="28" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A28" s="46"/>
+      <c r="A28" s="49"/>
       <c r="B28" s="25" t="s">
         <v>38</v>
       </c>
@@ -8583,7 +8583,7 @@
       </c>
     </row>
     <row r="29" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A29" s="46"/>
+      <c r="A29" s="49"/>
       <c r="B29" s="25" t="s">
         <v>39</v>
       </c>
@@ -8853,7 +8853,7 @@
       </c>
     </row>
     <row r="30" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A30" s="46"/>
+      <c r="A30" s="49"/>
       <c r="B30" s="25" t="s">
         <v>40</v>
       </c>
@@ -9132,7 +9132,7 @@
       </c>
     </row>
     <row r="31" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A31" s="46"/>
+      <c r="A31" s="49"/>
       <c r="B31" s="25" t="s">
         <v>41</v>
       </c>
@@ -9393,7 +9393,7 @@
       </c>
     </row>
     <row r="32" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A32" s="46"/>
+      <c r="A32" s="49"/>
       <c r="B32" s="25" t="s">
         <v>42</v>
       </c>
@@ -9654,7 +9654,7 @@
       </c>
     </row>
     <row r="33" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A33" s="46"/>
+      <c r="A33" s="49"/>
       <c r="B33" s="25"/>
       <c r="C33" s="26" t="s">
         <v>43</v>
@@ -9907,18 +9907,18 @@
       </c>
     </row>
     <row r="34" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A34" s="46"/>
+      <c r="A34" s="49"/>
       <c r="B34" s="25">
         <v>5</v>
       </c>
       <c r="C34" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D34" s="47">
+      <c r="D34" s="50">
         <f>J34-I34</f>
         <v>48</v>
       </c>
-      <c r="E34" s="47"/>
+      <c r="E34" s="50"/>
       <c r="F34" s="25"/>
       <c r="G34" s="25"/>
       <c r="H34" s="27" t="str">
@@ -10165,18 +10165,18 @@
       </c>
     </row>
     <row r="35" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A35" s="46"/>
+      <c r="A35" s="49"/>
       <c r="B35" s="25">
         <v>6</v>
       </c>
       <c r="C35" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="47">
+      <c r="D35" s="50">
         <f t="shared" ref="D35:D37" si="15">J35-I35</f>
         <v>21</v>
       </c>
-      <c r="E35" s="47"/>
+      <c r="E35" s="50"/>
       <c r="F35" s="25"/>
       <c r="G35" s="25"/>
       <c r="H35" s="27" t="str">
@@ -10423,18 +10423,18 @@
       </c>
     </row>
     <row r="36" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A36" s="46"/>
+      <c r="A36" s="49"/>
       <c r="B36" s="25">
         <v>7</v>
       </c>
       <c r="C36" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D36" s="47">
+      <c r="D36" s="50">
         <f t="shared" si="15"/>
         <v>14</v>
       </c>
-      <c r="E36" s="47"/>
+      <c r="E36" s="50"/>
       <c r="F36" s="25"/>
       <c r="G36" s="25"/>
       <c r="H36" s="27" t="str">
@@ -10681,18 +10681,18 @@
       </c>
     </row>
     <row r="37" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A37" s="46"/>
+      <c r="A37" s="49"/>
       <c r="B37" s="25">
         <v>8</v>
       </c>
       <c r="C37" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="47">
+      <c r="D37" s="50">
         <f t="shared" si="15"/>
         <v>48</v>
       </c>
-      <c r="E37" s="47"/>
+      <c r="E37" s="50"/>
       <c r="F37" s="25"/>
       <c r="G37" s="25"/>
       <c r="H37" s="27" t="str">
@@ -10939,7 +10939,7 @@
       </c>
     </row>
     <row r="38" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="46"/>
+      <c r="A38" s="49"/>
       <c r="B38" s="25"/>
       <c r="C38" s="26" t="s">
         <v>57</v>
@@ -11185,7 +11185,7 @@
       </c>
     </row>
     <row r="39" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="46"/>
+      <c r="A39" s="49"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26" t="s">
         <v>58</v>
@@ -11440,7 +11440,7 @@
       </c>
     </row>
     <row r="40" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="46"/>
+      <c r="A40" s="49"/>
       <c r="B40" s="25"/>
       <c r="C40" s="26" t="s">
         <v>56</v>
@@ -11687,12 +11687,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="K5:BP5"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
     <mergeCell ref="B5:C6"/>
     <mergeCell ref="D5:E6"/>
     <mergeCell ref="F5:G6"/>
@@ -11701,6 +11695,12 @@
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="K5:BP5"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B7:J40">
@@ -11914,8 +11914,8 @@
   </sheetPr>
   <dimension ref="A2:BP22"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11936,11 +11936,11 @@
       <c r="C2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="48">
+      <c r="D2" s="41">
         <v>45689</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:68" x14ac:dyDescent="0.35">
@@ -11948,11 +11948,11 @@
       <c r="C3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="49">
+      <c r="D3" s="42">
         <v>45961</v>
       </c>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:68" ht="5.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K4" s="8" cm="1">
@@ -12094,102 +12094,102 @@
       <c r="BP4" s="8"/>
     </row>
     <row r="5" spans="1:68" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="43" t="s">
+      <c r="C5" s="44"/>
+      <c r="D5" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43" t="s">
+      <c r="E5" s="45"/>
+      <c r="F5" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43" t="s">
+      <c r="G5" s="45"/>
+      <c r="H5" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="43" t="s">
+      <c r="J5" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="41" t="s">
+      <c r="K5" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="41"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="41"/>
-      <c r="U5" s="41"/>
-      <c r="V5" s="41"/>
-      <c r="W5" s="41"/>
-      <c r="X5" s="41"/>
-      <c r="Y5" s="41"/>
-      <c r="Z5" s="41"/>
-      <c r="AA5" s="41"/>
-      <c r="AB5" s="41"/>
-      <c r="AC5" s="41"/>
-      <c r="AD5" s="41"/>
-      <c r="AE5" s="41"/>
-      <c r="AF5" s="41"/>
-      <c r="AG5" s="41"/>
-      <c r="AH5" s="41"/>
-      <c r="AI5" s="41"/>
-      <c r="AJ5" s="41"/>
-      <c r="AK5" s="41"/>
-      <c r="AL5" s="41"/>
-      <c r="AM5" s="41"/>
-      <c r="AN5" s="41"/>
-      <c r="AO5" s="41"/>
-      <c r="AP5" s="41"/>
-      <c r="AQ5" s="41"/>
-      <c r="AR5" s="41"/>
-      <c r="AS5" s="41"/>
-      <c r="AT5" s="41"/>
-      <c r="AU5" s="41"/>
-      <c r="AV5" s="41"/>
-      <c r="AW5" s="41"/>
-      <c r="AX5" s="41"/>
-      <c r="AY5" s="41"/>
-      <c r="AZ5" s="41"/>
-      <c r="BA5" s="41"/>
-      <c r="BB5" s="41"/>
-      <c r="BC5" s="41"/>
-      <c r="BD5" s="41"/>
-      <c r="BE5" s="41"/>
-      <c r="BF5" s="41"/>
-      <c r="BG5" s="41"/>
-      <c r="BH5" s="41"/>
-      <c r="BI5" s="41"/>
-      <c r="BJ5" s="41"/>
-      <c r="BK5" s="41"/>
-      <c r="BL5" s="41"/>
-      <c r="BM5" s="41"/>
-      <c r="BN5" s="41"/>
-      <c r="BO5" s="41"/>
-      <c r="BP5" s="41"/>
+      <c r="L5" s="44"/>
+      <c r="M5" s="44"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="44"/>
+      <c r="Q5" s="44"/>
+      <c r="R5" s="44"/>
+      <c r="S5" s="44"/>
+      <c r="T5" s="44"/>
+      <c r="U5" s="44"/>
+      <c r="V5" s="44"/>
+      <c r="W5" s="44"/>
+      <c r="X5" s="44"/>
+      <c r="Y5" s="44"/>
+      <c r="Z5" s="44"/>
+      <c r="AA5" s="44"/>
+      <c r="AB5" s="44"/>
+      <c r="AC5" s="44"/>
+      <c r="AD5" s="44"/>
+      <c r="AE5" s="44"/>
+      <c r="AF5" s="44"/>
+      <c r="AG5" s="44"/>
+      <c r="AH5" s="44"/>
+      <c r="AI5" s="44"/>
+      <c r="AJ5" s="44"/>
+      <c r="AK5" s="44"/>
+      <c r="AL5" s="44"/>
+      <c r="AM5" s="44"/>
+      <c r="AN5" s="44"/>
+      <c r="AO5" s="44"/>
+      <c r="AP5" s="44"/>
+      <c r="AQ5" s="44"/>
+      <c r="AR5" s="44"/>
+      <c r="AS5" s="44"/>
+      <c r="AT5" s="44"/>
+      <c r="AU5" s="44"/>
+      <c r="AV5" s="44"/>
+      <c r="AW5" s="44"/>
+      <c r="AX5" s="44"/>
+      <c r="AY5" s="44"/>
+      <c r="AZ5" s="44"/>
+      <c r="BA5" s="44"/>
+      <c r="BB5" s="44"/>
+      <c r="BC5" s="44"/>
+      <c r="BD5" s="44"/>
+      <c r="BE5" s="44"/>
+      <c r="BF5" s="44"/>
+      <c r="BG5" s="44"/>
+      <c r="BH5" s="44"/>
+      <c r="BI5" s="44"/>
+      <c r="BJ5" s="44"/>
+      <c r="BK5" s="44"/>
+      <c r="BL5" s="44"/>
+      <c r="BM5" s="44"/>
+      <c r="BN5" s="44"/>
+      <c r="BO5" s="44"/>
+      <c r="BP5" s="44"/>
     </row>
     <row r="6" spans="1:68" s="9" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="46"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
       <c r="K6" s="1" t="str">
         <f>UPPER(IF(ISBLANK(K4), "", _xlfn.LET(
     _xlpm.date_of_previous_week, DATE(YEAR(D2),1,1) - WEEKDAY(DATE(YEAR(D2),1,1)) + 7*J4,
@@ -12432,7 +12432,7 @@
       </c>
     </row>
     <row r="7" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A7" s="46"/>
+      <c r="A7" s="49"/>
       <c r="B7" s="12"/>
       <c r="C7" s="15" t="s">
         <v>63</v>
@@ -12709,7 +12709,7 @@
       </c>
     </row>
     <row r="8" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A8" s="46"/>
+      <c r="A8" s="49"/>
       <c r="B8" s="12">
         <v>1</v>
       </c>
@@ -12717,26 +12717,32 @@
         <v>62</v>
       </c>
       <c r="D8" s="12">
-        <f>SUM(D9:D12)</f>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12">
-        <f>SUM(F9:F12)</f>
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="13">
         <f t="shared" ref="H8:H22" si="2">IF((LEN(B8) - LEN(SUBSTITUTE(B8, ".", ""))) = 2,  IF(ISBLANK(E8),"",IF(ISBLANK(G8),"",IF(E8=0,1,-(1-G8/E8)))), IF(ISBLANK(D8),"",IF(ISBLANK(F8),"",IF(D8=0,1,-(1-F8/D8)))))</f>
-        <v>0.53333333333333344</v>
+        <v>0.5</v>
       </c>
       <c r="I8" s="14">
-        <f>J7</f>
+        <f>IF(
+   ISNUMBER(FIND(".", B8)),
+   IF(
+   RIGHT(B8, 1) = "1",
+   I7,
+   J7
+   ),
+    J7
+)</f>
         <v>45691</v>
       </c>
       <c r="J8" s="16">
         <f>IF((LEN(B8) - LEN(SUBSTITUTE(B8, ".", ""))) = 2, WORKDAY(I8, IF(ISBLANK(G8),E8,G8)), WORKDAY(I8, IF(ISBLANK(F8),D8,F8)))</f>
-        <v>45722</v>
+        <v>45699</v>
       </c>
       <c r="K8" s="10" t="str">
         <f t="shared" ref="K8:Z14" si="3">_xlfn.LET(
@@ -12757,19 +12763,19 @@
       </c>
       <c r="M8" s="10">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="N8" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="O8" s="10">
-        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="P8" s="10">
-        <f t="shared" si="1"/>
-        <v>-1</v>
+      <c r="N8" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="O8" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="P8" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
       <c r="Q8" s="10" t="str">
         <f t="shared" si="1"/>
@@ -12999,7 +13005,7 @@
       </c>
     </row>
     <row r="9" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A9" s="46"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="12" t="s">
         <v>21</v>
       </c>
@@ -13019,44 +13025,52 @@
         <v>1</v>
       </c>
       <c r="I9" s="14">
-        <f t="shared" ref="I9:I22" si="6">J8</f>
-        <v>45722</v>
+        <f t="shared" ref="I9:I22" si="6">IF(
+   ISNUMBER(FIND(".", B9)),
+   IF(
+   RIGHT(B9, 1) = "1",
+   I8,
+   J8
+   ),
+    J8
+)</f>
+        <v>45691</v>
       </c>
       <c r="J9" s="16">
         <f t="shared" ref="J9:J22" si="7">IF((LEN(B9) - LEN(SUBSTITUTE(B9, ".", ""))) = 2, WORKDAY(I9, IF(ISBLANK(G9),E9,G9)), WORKDAY(I9, IF(ISBLANK(F9),D9,F9)))</f>
-        <v>45736</v>
+        <v>45705</v>
       </c>
       <c r="K9" s="10" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L9" s="10" t="str">
+      <c r="L9" s="10">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="M9" s="10" t="str">
+        <v>2</v>
+      </c>
+      <c r="M9" s="10">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="N9" s="10" t="str">
+        <v>-1</v>
+      </c>
+      <c r="N9" s="10">
         <f t="shared" si="3"/>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="O9" s="10" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="P9" s="10">
+      <c r="P9" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="Q9" s="10">
+        <v/>
+      </c>
+      <c r="Q9" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="R9" s="10">
+        <v/>
+      </c>
+      <c r="R9" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v/>
       </c>
       <c r="S9" s="10" t="str">
         <f t="shared" si="3"/>
@@ -13269,7 +13283,7 @@
       </c>
     </row>
     <row r="10" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A10" s="46"/>
+      <c r="A10" s="49"/>
       <c r="B10" s="12" t="s">
         <v>22</v>
       </c>
@@ -13292,11 +13306,11 @@
       </c>
       <c r="I10" s="14">
         <f t="shared" si="6"/>
-        <v>45736</v>
+        <v>45705</v>
       </c>
       <c r="J10" s="16">
         <f t="shared" si="7"/>
-        <v>45755</v>
+        <v>45722</v>
       </c>
       <c r="K10" s="10" t="str">
         <f t="shared" si="3"/>
@@ -13310,37 +13324,37 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="N10" s="10" t="str">
+      <c r="N10" s="10">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="O10" s="10" t="str">
+        <v>2</v>
+      </c>
+      <c r="O10" s="10">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="P10" s="10" t="str">
+        <v>2</v>
+      </c>
+      <c r="P10" s="10">
         <f t="shared" si="3"/>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="Q10" s="10" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="R10" s="10">
+      <c r="R10" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="S10" s="10">
+        <v/>
+      </c>
+      <c r="S10" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="T10" s="10">
+        <v/>
+      </c>
+      <c r="T10" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>-1</v>
-      </c>
-      <c r="U10" s="10">
+        <v/>
+      </c>
+      <c r="U10" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v/>
       </c>
       <c r="V10" s="10" t="str">
         <f t="shared" si="3"/>
@@ -13532,7 +13546,7 @@
       </c>
     </row>
     <row r="11" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A11" s="46"/>
+      <c r="A11" s="49"/>
       <c r="B11" s="12" t="s">
         <v>82</v>
       </c>
@@ -13553,11 +13567,11 @@
       </c>
       <c r="I11" s="14">
         <f t="shared" si="6"/>
-        <v>45755</v>
+        <v>45705</v>
       </c>
       <c r="J11" s="16">
         <f t="shared" si="7"/>
-        <v>45762</v>
+        <v>45712</v>
       </c>
       <c r="K11" s="10" t="str">
         <f t="shared" si="3"/>
@@ -13571,13 +13585,13 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="N11" s="10" t="str">
+      <c r="N11" s="10">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="O11" s="10" t="str">
+        <v>3</v>
+      </c>
+      <c r="O11" s="10">
         <f t="shared" si="3"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="P11" s="10" t="str">
         <f t="shared" si="3"/>
@@ -13599,13 +13613,13 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="U11" s="10">
+      <c r="U11" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="V11" s="10">
+        <v/>
+      </c>
+      <c r="V11" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v/>
       </c>
       <c r="W11" s="10" t="str">
         <f t="shared" si="3"/>
@@ -13793,7 +13807,7 @@
       </c>
     </row>
     <row r="12" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A12" s="46"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="12" t="s">
         <v>83</v>
       </c>
@@ -13814,11 +13828,11 @@
       </c>
       <c r="I12" s="14">
         <f t="shared" si="6"/>
-        <v>45762</v>
+        <v>45712</v>
       </c>
       <c r="J12" s="16">
         <f t="shared" si="7"/>
-        <v>45772</v>
+        <v>45722</v>
       </c>
       <c r="K12" s="10" t="str">
         <f t="shared" si="3"/>
@@ -13836,13 +13850,13 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="O12" s="10" t="str">
+      <c r="O12" s="10">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="P12" s="10" t="str">
+        <v>-1</v>
+      </c>
+      <c r="P12" s="10">
         <f t="shared" si="3"/>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="Q12" s="10" t="str">
         <f t="shared" si="3"/>
@@ -13864,13 +13878,13 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="V12" s="10">
+      <c r="V12" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>-1</v>
-      </c>
-      <c r="W12" s="10">
+        <v/>
+      </c>
+      <c r="W12" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v/>
       </c>
       <c r="X12" s="10" t="str">
         <f t="shared" si="3"/>
@@ -14054,7 +14068,7 @@
       </c>
     </row>
     <row r="13" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A13" s="46"/>
+      <c r="A13" s="49"/>
       <c r="B13" s="12">
         <v>2</v>
       </c>
@@ -14077,11 +14091,11 @@
       </c>
       <c r="I13" s="14">
         <f t="shared" si="6"/>
-        <v>45772</v>
+        <v>45722</v>
       </c>
       <c r="J13" s="16">
         <f t="shared" si="7"/>
-        <v>45775</v>
+        <v>45723</v>
       </c>
       <c r="K13" s="10" t="str">
         <f t="shared" si="3"/>
@@ -14103,9 +14117,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="P13" s="10" t="str">
+      <c r="P13" s="10">
         <f t="shared" si="3"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="Q13" s="10" t="str">
         <f t="shared" si="3"/>
@@ -14131,13 +14145,13 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="W13" s="10">
+      <c r="W13" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="X13" s="10">
+        <v/>
+      </c>
+      <c r="X13" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v/>
       </c>
       <c r="Y13" s="10" t="str">
         <f t="shared" si="3"/>
@@ -14317,7 +14331,7 @@
       </c>
     </row>
     <row r="14" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A14" s="46"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="12" t="s">
         <v>23</v>
       </c>
@@ -14338,11 +14352,11 @@
       </c>
       <c r="I14" s="14">
         <f t="shared" si="6"/>
-        <v>45775</v>
+        <v>45722</v>
       </c>
       <c r="J14" s="16">
         <f t="shared" si="7"/>
-        <v>45776</v>
+        <v>45723</v>
       </c>
       <c r="K14" s="10" t="str">
         <f t="shared" si="3"/>
@@ -14364,9 +14378,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="P14" s="10" t="str">
+      <c r="P14" s="10">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="Q14" s="10" t="str">
         <f t="shared" si="3"/>
@@ -14396,9 +14410,9 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="X14" s="10">
+      <c r="X14" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="Y14" s="10" t="str">
         <f t="shared" si="3"/>
@@ -14578,7 +14592,7 @@
       </c>
     </row>
     <row r="15" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A15" s="46"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="12"/>
       <c r="C15" s="15" t="s">
         <v>69</v>
@@ -14593,11 +14607,11 @@
       </c>
       <c r="I15" s="14">
         <f t="shared" si="6"/>
-        <v>45776</v>
+        <v>45723</v>
       </c>
       <c r="J15" s="16">
         <f t="shared" si="7"/>
-        <v>45776</v>
+        <v>45723</v>
       </c>
       <c r="K15" s="10" t="str">
         <f t="shared" ref="K15:Z22" si="9">_xlfn.LET(
@@ -14628,9 +14642,9 @@
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="P15" s="10" t="str">
+      <c r="P15" s="10">
         <f t="shared" si="9"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="Q15" s="10" t="str">
         <f t="shared" si="9"/>
@@ -14660,9 +14674,9 @@
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="X15" s="10">
+      <c r="X15" s="10" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="Y15" s="10" t="str">
         <f t="shared" si="9"/>
@@ -14869,7 +14883,7 @@
       </c>
     </row>
     <row r="16" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A16" s="46"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="12">
         <v>3</v>
       </c>
@@ -14890,11 +14904,11 @@
       </c>
       <c r="I16" s="14">
         <f t="shared" si="6"/>
-        <v>45776</v>
+        <v>45723</v>
       </c>
       <c r="J16" s="16">
         <f t="shared" si="7"/>
-        <v>45783</v>
+        <v>45730</v>
       </c>
       <c r="K16" s="10" t="str">
         <f t="shared" ref="K16:AP16" si="13">_xlfn.LET(
@@ -14925,13 +14939,13 @@
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="P16" s="10" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="Q16" s="10" t="str">
-        <f t="shared" si="13"/>
-        <v/>
+      <c r="P16" s="10">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="Q16" s="10">
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="R16" s="10" t="str">
         <f t="shared" si="13"/>
@@ -14957,13 +14971,13 @@
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="X16" s="10">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="Y16" s="10">
-        <f t="shared" si="13"/>
-        <v>1</v>
+      <c r="X16" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y16" s="10" t="str">
+        <f t="shared" si="13"/>
+        <v/>
       </c>
       <c r="Z16" s="10" t="str">
         <f t="shared" si="13"/>
@@ -15139,7 +15153,7 @@
       </c>
     </row>
     <row r="17" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A17" s="46"/>
+      <c r="A17" s="49"/>
       <c r="B17" s="12">
         <v>4</v>
       </c>
@@ -15158,11 +15172,11 @@
       </c>
       <c r="I17" s="14">
         <f t="shared" si="6"/>
-        <v>45783</v>
+        <v>45730</v>
       </c>
       <c r="J17" s="16">
         <f t="shared" si="7"/>
-        <v>45811</v>
+        <v>45758</v>
       </c>
       <c r="K17" s="10" t="str">
         <f t="shared" si="9"/>
@@ -15188,25 +15202,25 @@
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="Q17" s="10" t="str">
+      <c r="Q17" s="10">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="R17" s="10" t="str">
+        <v>1</v>
+      </c>
+      <c r="R17" s="10">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="S17" s="10" t="str">
+        <v>1</v>
+      </c>
+      <c r="S17" s="10">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="T17" s="10" t="str">
+        <v>1</v>
+      </c>
+      <c r="T17" s="10">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="U17" s="10" t="str">
+        <v>1</v>
+      </c>
+      <c r="U17" s="10">
         <f t="shared" si="9"/>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="V17" s="10" t="str">
         <f t="shared" si="9"/>
@@ -15220,25 +15234,25 @@
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="Y17" s="10">
+      <c r="Y17" s="10" t="str">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="Z17" s="10">
+        <v/>
+      </c>
+      <c r="Z17" s="10" t="str">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="AA17" s="10">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AB17" s="10">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AC17" s="10">
-        <f t="shared" si="10"/>
-        <v>-1</v>
+        <v/>
+      </c>
+      <c r="AA17" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AB17" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AC17" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
       </c>
       <c r="AD17" s="10" t="str">
         <f t="shared" si="10"/>
@@ -15398,7 +15412,7 @@
       </c>
     </row>
     <row r="18" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A18" s="46"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="12">
         <v>5</v>
       </c>
@@ -15417,11 +15431,11 @@
       </c>
       <c r="I18" s="14">
         <f t="shared" si="6"/>
-        <v>45811</v>
+        <v>45758</v>
       </c>
       <c r="J18" s="16">
         <f t="shared" si="7"/>
-        <v>45859</v>
+        <v>45806</v>
       </c>
       <c r="K18" s="10" t="str">
         <f t="shared" si="9"/>
@@ -15463,69 +15477,69 @@
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="U18" s="10" t="str">
+      <c r="U18" s="10">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="V18" s="10" t="str">
+        <v>1</v>
+      </c>
+      <c r="V18" s="10">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="W18" s="10" t="str">
+        <v>1</v>
+      </c>
+      <c r="W18" s="10">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="X18" s="10" t="str">
+        <v>1</v>
+      </c>
+      <c r="X18" s="10">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="Y18" s="10" t="str">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="10">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="Z18" s="10" t="str">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="10">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AA18" s="10" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AB18" s="10" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AC18" s="10">
-        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="AD18" s="10">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AE18" s="10">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AF18" s="10">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AG18" s="10">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AH18" s="10">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AI18" s="10">
+      <c r="AA18" s="10">
         <f t="shared" si="10"/>
         <v>-1</v>
       </c>
-      <c r="AJ18" s="10">
+      <c r="AB18" s="10">
         <f t="shared" si="10"/>
         <v>-1</v>
+      </c>
+      <c r="AC18" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AD18" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AE18" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AF18" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AG18" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AH18" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AI18" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AJ18" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
       </c>
       <c r="AK18" s="10" t="str">
         <f t="shared" si="10"/>
@@ -15657,7 +15671,7 @@
       </c>
     </row>
     <row r="19" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A19" s="46"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="12">
         <v>6</v>
       </c>
@@ -15676,11 +15690,11 @@
       </c>
       <c r="I19" s="14">
         <f t="shared" si="6"/>
-        <v>45859</v>
+        <v>45806</v>
       </c>
       <c r="J19" s="16">
         <f t="shared" si="7"/>
-        <v>45875</v>
+        <v>45824</v>
       </c>
       <c r="K19" s="10" t="str">
         <f t="shared" si="9"/>
@@ -15750,21 +15764,21 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AB19" s="10" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AC19" s="10" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AD19" s="10" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AE19" s="10" t="str">
-        <f t="shared" si="10"/>
-        <v/>
+      <c r="AB19" s="10">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AC19" s="10">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AD19" s="10">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="AE19" s="10">
+        <f t="shared" si="10"/>
+        <v>-1</v>
       </c>
       <c r="AF19" s="10" t="str">
         <f t="shared" si="10"/>
@@ -15782,17 +15796,17 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AJ19" s="10">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AK19" s="10">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="AL19" s="10">
-        <f t="shared" si="11"/>
-        <v>-1</v>
+      <c r="AJ19" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AK19" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AL19" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v/>
       </c>
       <c r="AM19" s="10" t="str">
         <f t="shared" si="11"/>
@@ -15932,11 +15946,11 @@
       </c>
       <c r="I20" s="14">
         <f t="shared" si="6"/>
-        <v>45875</v>
+        <v>45824</v>
       </c>
       <c r="J20" s="16">
         <f t="shared" si="7"/>
-        <v>45876</v>
+        <v>45825</v>
       </c>
       <c r="K20" s="10" t="str">
         <f t="shared" ref="K20:AP20" si="14">_xlfn.LET(
@@ -16027,9 +16041,9 @@
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="AE20" s="10" t="str">
-        <f t="shared" si="14"/>
-        <v/>
+      <c r="AE20" s="10">
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="AF20" s="10" t="str">
         <f t="shared" si="14"/>
@@ -16055,9 +16069,9 @@
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="AL20" s="10">
-        <f t="shared" si="14"/>
-        <v>0</v>
+      <c r="AL20" s="10" t="str">
+        <f t="shared" si="14"/>
+        <v/>
       </c>
       <c r="AM20" s="10" t="str">
         <f t="shared" si="14"/>
@@ -16202,11 +16216,11 @@
       </c>
       <c r="I21" s="14">
         <f t="shared" si="6"/>
-        <v>45876</v>
+        <v>45825</v>
       </c>
       <c r="J21" s="16">
         <f t="shared" si="7"/>
-        <v>45880</v>
+        <v>45827</v>
       </c>
       <c r="K21" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16288,9 +16302,9 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AE21" s="10" t="str">
-        <f t="shared" si="10"/>
-        <v/>
+      <c r="AE21" s="10">
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="AF21" s="10" t="str">
         <f t="shared" si="10"/>
@@ -16316,13 +16330,13 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AL21" s="10">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AM21" s="10">
-        <f t="shared" si="11"/>
-        <v>-1</v>
+      <c r="AL21" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="AM21" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v/>
       </c>
       <c r="AN21" s="10" t="str">
         <f t="shared" si="11"/>
@@ -16463,11 +16477,11 @@
       </c>
       <c r="I22" s="14">
         <f t="shared" si="6"/>
-        <v>45880</v>
+        <v>45827</v>
       </c>
       <c r="J22" s="16">
         <f t="shared" si="7"/>
-        <v>45883</v>
+        <v>45832</v>
       </c>
       <c r="K22" s="10" t="str">
         <f t="shared" si="9"/>
@@ -16549,13 +16563,13 @@
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="AE22" s="10" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="AF22" s="10" t="str">
-        <f t="shared" si="10"/>
-        <v/>
+      <c r="AE22" s="10">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AF22" s="10">
+        <f t="shared" si="10"/>
+        <v>-1</v>
       </c>
       <c r="AG22" s="10" t="str">
         <f t="shared" si="10"/>
@@ -16581,9 +16595,9 @@
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="AM22" s="10">
-        <f t="shared" si="11"/>
-        <v>0</v>
+      <c r="AM22" s="10" t="str">
+        <f t="shared" si="11"/>
+        <v/>
       </c>
       <c r="AN22" s="10" t="str">
         <f t="shared" si="11"/>
@@ -16700,16 +16714,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:BP5"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A5:A19"/>
     <mergeCell ref="B5:C6"/>
     <mergeCell ref="D5:E6"/>
     <mergeCell ref="F5:G6"/>
     <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:BP5"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B7:J22">

</xml_diff>